<commit_message>
Took measurements for slices
</commit_message>
<xml_diff>
--- a/Paxinos & Watson/SliceData.xlsx
+++ b/Paxinos & Watson/SliceData.xlsx
@@ -373,8 +373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,8 +386,8 @@
     <col min="6" max="6" width="18.85546875" customWidth="1"/>
     <col min="7" max="7" width="24" customWidth="1"/>
     <col min="8" max="8" width="25" customWidth="1"/>
-    <col min="9" max="9" width="50.5703125" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
+    <col min="10" max="10" width="50.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -416,310 +416,2050 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>0.48</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>3.875</v>
+      </c>
+      <c r="E2">
+        <f>C2+2*D2</f>
+        <v>17.75</v>
+      </c>
+      <c r="F2">
+        <v>8</v>
+      </c>
+      <c r="G2">
+        <v>0.875</v>
+      </c>
+      <c r="H2">
+        <v>7.625</v>
+      </c>
+      <c r="I2">
+        <f>F2+G2+H2</f>
+        <v>16.5</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>0.48</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>3.875</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E61" si="0">C3+2*D3</f>
+        <v>17.75</v>
+      </c>
+      <c r="F3">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>0.875</v>
+      </c>
+      <c r="H3">
+        <v>7.625</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I61" si="1">F3+G3+H3</f>
+        <v>16.5</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4">
+        <v>0.48</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>3.875</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F4">
+        <v>8</v>
+      </c>
+      <c r="G4">
+        <v>0.875</v>
+      </c>
+      <c r="H4">
+        <v>7.625</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5">
+        <v>0.48</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>3.875</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F5">
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>0.875</v>
+      </c>
+      <c r="H5">
+        <v>7.625</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6">
+        <v>0.48</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>3.875</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F6">
+        <v>8</v>
+      </c>
+      <c r="G6">
+        <v>0.875</v>
+      </c>
+      <c r="H6">
+        <v>7.625</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7">
+        <v>0.48</v>
+      </c>
+      <c r="C7">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>1.875</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>0.875</v>
+      </c>
+      <c r="H7">
+        <v>5.625</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8">
+        <v>0.48</v>
+      </c>
+      <c r="C8">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>1.875</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>0.875</v>
+      </c>
+      <c r="H8">
+        <v>5.625</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9">
+        <v>0.48</v>
+      </c>
+      <c r="C9">
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <v>1.875</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>0.875</v>
+      </c>
+      <c r="H9">
+        <v>5.625</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10">
+        <v>0.48</v>
+      </c>
+      <c r="C10">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>1.875</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <v>0.875</v>
+      </c>
+      <c r="H10">
+        <v>5.625</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11">
+        <v>0.24</v>
+      </c>
+      <c r="C11">
+        <v>14</v>
+      </c>
+      <c r="D11">
+        <v>1.875</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11">
+        <v>0.875</v>
+      </c>
+      <c r="H11">
+        <v>5.625</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
+      </c>
+      <c r="B12">
+        <v>0.24</v>
+      </c>
+      <c r="C12">
+        <v>14</v>
+      </c>
+      <c r="D12">
+        <v>1.875</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>0.875</v>
+      </c>
+      <c r="H12">
+        <v>5.625</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13">
+        <v>0.24</v>
+      </c>
+      <c r="C13">
+        <v>16</v>
+      </c>
+      <c r="D13">
+        <v>0.875</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F13">
+        <v>11</v>
+      </c>
+      <c r="G13">
+        <v>0.875</v>
+      </c>
+      <c r="H13">
+        <v>4.625</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J13">
+        <v>-1</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14">
+        <v>0.24</v>
+      </c>
+      <c r="C14">
+        <v>16</v>
+      </c>
+      <c r="D14">
+        <v>0.875</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F14">
+        <v>11</v>
+      </c>
+      <c r="G14">
+        <v>0.875</v>
+      </c>
+      <c r="H14">
+        <v>4.625</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J14">
+        <v>-1</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15">
+        <v>0.12</v>
+      </c>
+      <c r="C15">
+        <v>16</v>
+      </c>
+      <c r="D15">
+        <v>0.875</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F15">
+        <v>11</v>
+      </c>
+      <c r="G15">
+        <v>0.875</v>
+      </c>
+      <c r="H15">
+        <v>4.625</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J15">
+        <v>-1</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>0.12</v>
+      </c>
+      <c r="C16">
+        <v>16</v>
+      </c>
+      <c r="D16">
+        <v>0.875</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F16">
+        <v>11</v>
+      </c>
+      <c r="G16">
+        <v>0.875</v>
+      </c>
+      <c r="H16">
+        <v>4.625</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J16">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>0.12</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <v>0.875</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F17">
+        <v>11</v>
+      </c>
+      <c r="G17">
+        <v>0.875</v>
+      </c>
+      <c r="H17">
+        <v>4.625</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J17">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>0.12</v>
+      </c>
+      <c r="C18">
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <v>0.875</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F18">
+        <v>11</v>
+      </c>
+      <c r="G18">
+        <v>0.875</v>
+      </c>
+      <c r="H18">
+        <v>4.625</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J18">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>0.12</v>
+      </c>
+      <c r="C19">
+        <v>16</v>
+      </c>
+      <c r="D19">
+        <v>0.875</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F19">
+        <v>11</v>
+      </c>
+      <c r="G19">
+        <v>0.875</v>
+      </c>
+      <c r="H19">
+        <v>4.625</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J19">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>0.12</v>
+      </c>
+      <c r="C20">
+        <v>16</v>
+      </c>
+      <c r="D20">
+        <v>0.875</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F20">
+        <v>11</v>
+      </c>
+      <c r="G20">
+        <v>0.875</v>
+      </c>
+      <c r="H20">
+        <v>4.625</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J20">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>0.12</v>
+      </c>
+      <c r="C21">
+        <v>16</v>
+      </c>
+      <c r="D21">
+        <v>0.875</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F21">
+        <v>11</v>
+      </c>
+      <c r="G21">
+        <v>0.875</v>
+      </c>
+      <c r="H21">
+        <v>4.625</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>0.12</v>
+      </c>
+      <c r="C22">
+        <v>16</v>
+      </c>
+      <c r="D22">
+        <v>0.875</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F22">
+        <v>11</v>
+      </c>
+      <c r="G22">
+        <v>0.875</v>
+      </c>
+      <c r="H22">
+        <v>4.625</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J22">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>0.12</v>
+      </c>
+      <c r="C23">
+        <v>16</v>
+      </c>
+      <c r="D23">
+        <v>0.875</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F23">
+        <v>11</v>
+      </c>
+      <c r="G23">
+        <v>0.875</v>
+      </c>
+      <c r="H23">
+        <v>4.625</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J23">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>0.12</v>
+      </c>
+      <c r="C24">
+        <v>16</v>
+      </c>
+      <c r="D24">
+        <v>0.875</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F24">
+        <v>11</v>
+      </c>
+      <c r="G24">
+        <v>0.875</v>
+      </c>
+      <c r="H24">
+        <v>4.625</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J24">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>0.12</v>
+      </c>
+      <c r="C25">
+        <v>16</v>
+      </c>
+      <c r="D25">
+        <v>0.875</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F25">
+        <v>11</v>
+      </c>
+      <c r="G25">
+        <v>0.875</v>
+      </c>
+      <c r="H25">
+        <v>4.625</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>0.12</v>
+      </c>
+      <c r="C26">
+        <v>16</v>
+      </c>
+      <c r="D26">
+        <v>0.875</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F26">
+        <v>11</v>
+      </c>
+      <c r="G26">
+        <v>0.875</v>
+      </c>
+      <c r="H26">
+        <v>4.625</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J26">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>0.12</v>
+      </c>
+      <c r="C27">
+        <v>16</v>
+      </c>
+      <c r="D27">
+        <v>0.875</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F27">
+        <v>11</v>
+      </c>
+      <c r="G27">
+        <v>0.875</v>
+      </c>
+      <c r="H27">
+        <v>4.625</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J27">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>0.12</v>
+      </c>
+      <c r="C28">
+        <v>16</v>
+      </c>
+      <c r="D28">
+        <v>0.875</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F28">
+        <v>11</v>
+      </c>
+      <c r="G28">
+        <v>0.875</v>
+      </c>
+      <c r="H28">
+        <v>4.625</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J28">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>0.12</v>
+      </c>
+      <c r="C29">
+        <v>16</v>
+      </c>
+      <c r="D29">
+        <v>0.875</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F29">
+        <v>11</v>
+      </c>
+      <c r="G29">
+        <v>0.875</v>
+      </c>
+      <c r="H29">
+        <v>4.625</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J29">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>0.12</v>
+      </c>
+      <c r="C30">
+        <v>16</v>
+      </c>
+      <c r="D30">
+        <v>0.875</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F30">
+        <v>11</v>
+      </c>
+      <c r="G30">
+        <v>0.875</v>
+      </c>
+      <c r="H30">
+        <v>4.625</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J30">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>0.12</v>
+      </c>
+      <c r="C31">
+        <v>16</v>
+      </c>
+      <c r="D31">
+        <v>0.875</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F31">
+        <v>11</v>
+      </c>
+      <c r="G31">
+        <v>0.875</v>
+      </c>
+      <c r="H31">
+        <v>4.625</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J31">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>0.12</v>
+      </c>
+      <c r="C32">
+        <v>16</v>
+      </c>
+      <c r="D32">
+        <v>0.875</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F32">
+        <v>11</v>
+      </c>
+      <c r="G32">
+        <v>0.875</v>
+      </c>
+      <c r="H32">
+        <v>4.625</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J32">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>0.12</v>
+      </c>
+      <c r="C33">
+        <v>16</v>
+      </c>
+      <c r="D33">
+        <v>0.875</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F33">
+        <v>11</v>
+      </c>
+      <c r="G33">
+        <v>0.875</v>
+      </c>
+      <c r="H33">
+        <v>4.625</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J33">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>0.12</v>
+      </c>
+      <c r="C34">
+        <v>16</v>
+      </c>
+      <c r="D34">
+        <v>0.875</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F34">
+        <v>11</v>
+      </c>
+      <c r="G34">
+        <v>0.875</v>
+      </c>
+      <c r="H34">
+        <v>4.625</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J34">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>0.12</v>
+      </c>
+      <c r="C35">
+        <v>16</v>
+      </c>
+      <c r="D35">
+        <v>0.875</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F35">
+        <v>11</v>
+      </c>
+      <c r="G35">
+        <v>0.875</v>
+      </c>
+      <c r="H35">
+        <v>4.625</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J35">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>0.12</v>
+      </c>
+      <c r="C36">
+        <v>16</v>
+      </c>
+      <c r="D36">
+        <v>0.875</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F36">
+        <v>11</v>
+      </c>
+      <c r="G36">
+        <v>0.875</v>
+      </c>
+      <c r="H36">
+        <v>4.625</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>0.12</v>
+      </c>
+      <c r="C37">
+        <v>16</v>
+      </c>
+      <c r="D37">
+        <v>0.875</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F37">
+        <v>11</v>
+      </c>
+      <c r="G37">
+        <v>0.875</v>
+      </c>
+      <c r="H37">
+        <v>4.625</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>0.12</v>
+      </c>
+      <c r="C38">
+        <v>16</v>
+      </c>
+      <c r="D38">
+        <v>0.875</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F38">
+        <v>11</v>
+      </c>
+      <c r="G38">
+        <v>0.875</v>
+      </c>
+      <c r="H38">
+        <v>4.625</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>0.12</v>
+      </c>
+      <c r="C39">
+        <v>16</v>
+      </c>
+      <c r="D39">
+        <v>0.875</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F39">
+        <v>11</v>
+      </c>
+      <c r="G39">
+        <v>0.875</v>
+      </c>
+      <c r="H39">
+        <v>4.625</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>0.12</v>
+      </c>
+      <c r="C40">
+        <v>16</v>
+      </c>
+      <c r="D40">
+        <v>0.875</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F40">
+        <v>11</v>
+      </c>
+      <c r="G40">
+        <v>0.875</v>
+      </c>
+      <c r="H40">
+        <v>4.625</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>0.12</v>
+      </c>
+      <c r="C41">
+        <v>16</v>
+      </c>
+      <c r="D41">
+        <v>0.875</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F41">
+        <v>11</v>
+      </c>
+      <c r="G41">
+        <v>0.875</v>
+      </c>
+      <c r="H41">
+        <v>4.625</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>0.12</v>
+      </c>
+      <c r="C42">
+        <v>16</v>
+      </c>
+      <c r="D42">
+        <v>0.875</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F42">
+        <v>11</v>
+      </c>
+      <c r="G42">
+        <v>0.875</v>
+      </c>
+      <c r="H42">
+        <v>4.625</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>0.12</v>
+      </c>
+      <c r="C43">
+        <v>16</v>
+      </c>
+      <c r="D43">
+        <v>0.875</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F43">
+        <v>11</v>
+      </c>
+      <c r="G43">
+        <v>0.875</v>
+      </c>
+      <c r="H43">
+        <v>4.625</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>0.12</v>
+      </c>
+      <c r="C44">
+        <v>16</v>
+      </c>
+      <c r="D44">
+        <v>0.875</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F44">
+        <v>11</v>
+      </c>
+      <c r="G44">
+        <v>0.875</v>
+      </c>
+      <c r="H44">
+        <v>4.625</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>0.12</v>
+      </c>
+      <c r="C45">
+        <v>16</v>
+      </c>
+      <c r="D45">
+        <v>0.875</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F45">
+        <v>11</v>
+      </c>
+      <c r="G45">
+        <v>0.875</v>
+      </c>
+      <c r="H45">
+        <v>4.625</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>0.12</v>
+      </c>
+      <c r="C46">
+        <v>16</v>
+      </c>
+      <c r="D46">
+        <v>0.875</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F46">
+        <v>11</v>
+      </c>
+      <c r="G46">
+        <v>0.875</v>
+      </c>
+      <c r="H46">
+        <v>4.625</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>0.16</v>
+      </c>
+      <c r="C47">
+        <v>16</v>
+      </c>
+      <c r="D47">
+        <v>0.875</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F47">
+        <v>11</v>
+      </c>
+      <c r="G47">
+        <v>0.875</v>
+      </c>
+      <c r="H47">
+        <v>4.625</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>0.08</v>
+      </c>
+      <c r="C48">
+        <v>16</v>
+      </c>
+      <c r="D48">
+        <v>0.875</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F48">
+        <v>11</v>
+      </c>
+      <c r="G48">
+        <v>0.875</v>
+      </c>
+      <c r="H48">
+        <v>4.625</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>0.12</v>
+      </c>
+      <c r="C49">
+        <v>16</v>
+      </c>
+      <c r="D49">
+        <v>0.875</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F49">
+        <v>11</v>
+      </c>
+      <c r="G49">
+        <v>0.875</v>
+      </c>
+      <c r="H49">
+        <v>4.625</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>0.12</v>
+      </c>
+      <c r="C50">
+        <v>16</v>
+      </c>
+      <c r="D50">
+        <v>0.875</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F50">
+        <v>11</v>
+      </c>
+      <c r="G50">
+        <v>0.875</v>
+      </c>
+      <c r="H50">
+        <v>4.625</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>0.12</v>
+      </c>
+      <c r="C51">
+        <v>16</v>
+      </c>
+      <c r="D51">
+        <v>0.875</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F51">
+        <v>11</v>
+      </c>
+      <c r="G51">
+        <v>0.875</v>
+      </c>
+      <c r="H51">
+        <v>4.625</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>0.12</v>
+      </c>
+      <c r="C52">
+        <v>16</v>
+      </c>
+      <c r="D52">
+        <v>0.875</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F52">
+        <v>11</v>
+      </c>
+      <c r="G52">
+        <v>0.875</v>
+      </c>
+      <c r="H52">
+        <v>4.625</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>0.12</v>
+      </c>
+      <c r="C53">
+        <v>16</v>
+      </c>
+      <c r="D53">
+        <v>0.875</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F53">
+        <v>11</v>
+      </c>
+      <c r="G53">
+        <v>0.875</v>
+      </c>
+      <c r="H53">
+        <v>4.625</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>0.12</v>
+      </c>
+      <c r="C54">
+        <v>16</v>
+      </c>
+      <c r="D54">
+        <v>0.875</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F54">
+        <v>11</v>
+      </c>
+      <c r="G54">
+        <v>0.875</v>
+      </c>
+      <c r="H54">
+        <v>4.625</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>0.12</v>
+      </c>
+      <c r="C55">
+        <v>16</v>
+      </c>
+      <c r="D55">
+        <v>0.875</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F55">
+        <v>11</v>
+      </c>
+      <c r="G55">
+        <v>0.875</v>
+      </c>
+      <c r="H55">
+        <v>4.625</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>0.12</v>
+      </c>
+      <c r="C56">
+        <v>16</v>
+      </c>
+      <c r="D56">
+        <v>0.875</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F56">
+        <v>11</v>
+      </c>
+      <c r="G56">
+        <v>0.875</v>
+      </c>
+      <c r="H56">
+        <v>4.625</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>0.16</v>
+      </c>
+      <c r="C57">
+        <v>16</v>
+      </c>
+      <c r="D57">
+        <v>0.875</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F57">
+        <v>11</v>
+      </c>
+      <c r="G57">
+        <v>0.875</v>
+      </c>
+      <c r="H57">
+        <v>4.625</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>0.08</v>
+      </c>
+      <c r="C58">
+        <v>16</v>
+      </c>
+      <c r="D58">
+        <v>0.875</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F58">
+        <v>11</v>
+      </c>
+      <c r="G58">
+        <v>0.875</v>
+      </c>
+      <c r="H58">
+        <v>4.625</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>0.12</v>
+      </c>
+      <c r="C59">
+        <v>16</v>
+      </c>
+      <c r="D59">
+        <v>0.875</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F59">
+        <v>11</v>
+      </c>
+      <c r="G59">
+        <v>0.875</v>
+      </c>
+      <c r="H59">
+        <v>4.625</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <v>0.12</v>
+      </c>
+      <c r="C60">
+        <v>16</v>
+      </c>
+      <c r="D60">
+        <v>0.875</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F60">
+        <v>11</v>
+      </c>
+      <c r="G60">
+        <v>0.875</v>
+      </c>
+      <c r="H60">
+        <v>4.625</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
+      </c>
+      <c r="B61">
+        <v>0.12</v>
+      </c>
+      <c r="C61">
+        <v>16</v>
+      </c>
+      <c r="D61">
+        <v>0.875</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="F61">
+        <v>11</v>
+      </c>
+      <c r="G61">
+        <v>0.875</v>
+      </c>
+      <c r="H61">
+        <v>4.625</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Introduced region data storage cell
</commit_message>
<xml_diff>
--- a/Paxinos & Watson/SliceData.xlsx
+++ b/Paxinos & Watson/SliceData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erica.nordin\Documents\3DFrontalCortex\Paxinos &amp; Watson\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Fall 2017 Co-op\3DFrontalCortex\Paxinos &amp; Watson\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Figure #</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Total Height (mm)</t>
+  </si>
+  <si>
+    <t>Bregma (mm)</t>
   </si>
 </sst>
 </file>
@@ -380,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,7 +402,7 @@
     <col min="10" max="10" width="50.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -407,31 +410,34 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -439,33 +445,36 @@
         <v>0.48</v>
       </c>
       <c r="C2">
+        <v>7.56</v>
+      </c>
+      <c r="D2">
         <v>10</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>3.875</v>
       </c>
-      <c r="E2">
-        <f>C2+2*D2</f>
-        <v>17.75</v>
-      </c>
       <c r="F2">
+        <f>D2+2*E2</f>
+        <v>17.75</v>
+      </c>
+      <c r="G2">
         <v>8</v>
       </c>
-      <c r="G2">
-        <v>0.875</v>
-      </c>
       <c r="H2">
+        <v>0.875</v>
+      </c>
+      <c r="I2">
         <v>7.625</v>
       </c>
-      <c r="I2">
-        <f>F2+G2+H2</f>
-        <v>16.5</v>
-      </c>
       <c r="J2">
+        <f>G2+H2+I2</f>
+        <v>16.5</v>
+      </c>
+      <c r="K2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -473,33 +482,37 @@
         <v>0.48</v>
       </c>
       <c r="C3">
+        <f>C2-B2</f>
+        <v>7.08</v>
+      </c>
+      <c r="D3">
         <v>10</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>3.875</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E61" si="0">C3+2*D3</f>
-        <v>17.75</v>
-      </c>
       <c r="F3">
+        <f t="shared" ref="F3:F61" si="0">D3+2*E3</f>
+        <v>17.75</v>
+      </c>
+      <c r="G3">
         <v>8</v>
       </c>
-      <c r="G3">
-        <v>0.875</v>
-      </c>
       <c r="H3">
+        <v>0.875</v>
+      </c>
+      <c r="I3">
         <v>7.625</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I61" si="1">F3+G3+H3</f>
-        <v>16.5</v>
-      </c>
       <c r="J3">
+        <f t="shared" ref="J3:J61" si="1">G3+H3+I3</f>
+        <v>16.5</v>
+      </c>
+      <c r="K3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -507,33 +520,37 @@
         <v>0.48</v>
       </c>
       <c r="C4">
+        <f t="shared" ref="C4:C61" si="2">C3-B3</f>
+        <v>6.6</v>
+      </c>
+      <c r="D4">
         <v>10</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>3.875</v>
       </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
-      </c>
       <c r="F4">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="G4">
         <v>8</v>
       </c>
-      <c r="G4">
-        <v>0.875</v>
-      </c>
       <c r="H4">
+        <v>0.875</v>
+      </c>
+      <c r="I4">
         <v>7.625</v>
       </c>
-      <c r="I4">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
-      </c>
       <c r="J4">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -541,33 +558,37 @@
         <v>0.48</v>
       </c>
       <c r="C5">
+        <f t="shared" si="2"/>
+        <v>6.1199999999999992</v>
+      </c>
+      <c r="D5">
         <v>10</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>3.875</v>
       </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
-      </c>
       <c r="F5">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="G5">
         <v>8</v>
       </c>
-      <c r="G5">
-        <v>0.875</v>
-      </c>
       <c r="H5">
+        <v>0.875</v>
+      </c>
+      <c r="I5">
         <v>7.625</v>
       </c>
-      <c r="I5">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
-      </c>
       <c r="J5">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -575,33 +596,37 @@
         <v>0.48</v>
       </c>
       <c r="C6">
+        <f t="shared" si="2"/>
+        <v>5.6399999999999988</v>
+      </c>
+      <c r="D6">
         <v>10</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>3.875</v>
       </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
-      </c>
       <c r="F6">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="G6">
         <v>8</v>
       </c>
-      <c r="G6">
-        <v>0.875</v>
-      </c>
       <c r="H6">
+        <v>0.875</v>
+      </c>
+      <c r="I6">
         <v>7.625</v>
       </c>
-      <c r="I6">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
-      </c>
       <c r="J6">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -609,33 +634,37 @@
         <v>0.48</v>
       </c>
       <c r="C7">
+        <f t="shared" si="2"/>
+        <v>5.1599999999999984</v>
+      </c>
+      <c r="D7">
         <v>14</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>1.875</v>
       </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
-      </c>
       <c r="F7">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="G7">
         <v>10</v>
       </c>
-      <c r="G7">
-        <v>0.875</v>
-      </c>
       <c r="H7">
+        <v>0.875</v>
+      </c>
+      <c r="I7">
         <v>5.625</v>
       </c>
-      <c r="I7">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
-      </c>
       <c r="J7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -643,33 +672,37 @@
         <v>0.48</v>
       </c>
       <c r="C8">
+        <f t="shared" si="2"/>
+        <v>4.6799999999999979</v>
+      </c>
+      <c r="D8">
         <v>14</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>1.875</v>
       </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
-      </c>
       <c r="F8">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="G8">
         <v>10</v>
       </c>
-      <c r="G8">
-        <v>0.875</v>
-      </c>
       <c r="H8">
+        <v>0.875</v>
+      </c>
+      <c r="I8">
         <v>5.625</v>
       </c>
-      <c r="I8">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
-      </c>
       <c r="J8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -677,33 +710,37 @@
         <v>0.48</v>
       </c>
       <c r="C9">
+        <f t="shared" si="2"/>
+        <v>4.1999999999999975</v>
+      </c>
+      <c r="D9">
         <v>14</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>1.875</v>
       </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
-      </c>
       <c r="F9">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="G9">
         <v>10</v>
       </c>
-      <c r="G9">
-        <v>0.875</v>
-      </c>
       <c r="H9">
+        <v>0.875</v>
+      </c>
+      <c r="I9">
         <v>5.625</v>
       </c>
-      <c r="I9">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
-      </c>
       <c r="J9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -711,33 +748,37 @@
         <v>0.48</v>
       </c>
       <c r="C10">
+        <f t="shared" si="2"/>
+        <v>3.7199999999999975</v>
+      </c>
+      <c r="D10">
         <v>14</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>1.875</v>
       </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
-      </c>
       <c r="F10">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="G10">
         <v>10</v>
       </c>
-      <c r="G10">
-        <v>0.875</v>
-      </c>
       <c r="H10">
+        <v>0.875</v>
+      </c>
+      <c r="I10">
         <v>5.625</v>
       </c>
-      <c r="I10">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
-      </c>
       <c r="J10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -745,33 +786,37 @@
         <v>0.24</v>
       </c>
       <c r="C11">
+        <f t="shared" si="2"/>
+        <v>3.2399999999999975</v>
+      </c>
+      <c r="D11">
         <v>14</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>1.875</v>
       </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
-      </c>
       <c r="F11">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="G11">
         <v>10</v>
       </c>
-      <c r="G11">
-        <v>0.875</v>
-      </c>
       <c r="H11">
+        <v>0.875</v>
+      </c>
+      <c r="I11">
         <v>5.625</v>
       </c>
-      <c r="I11">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
-      </c>
       <c r="J11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -779,33 +824,37 @@
         <v>0.24</v>
       </c>
       <c r="C12">
+        <f t="shared" si="2"/>
+        <v>2.9999999999999973</v>
+      </c>
+      <c r="D12">
         <v>14</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>1.875</v>
       </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
-      </c>
       <c r="F12">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="G12">
         <v>10</v>
       </c>
-      <c r="G12">
-        <v>0.875</v>
-      </c>
       <c r="H12">
+        <v>0.875</v>
+      </c>
+      <c r="I12">
         <v>5.625</v>
       </c>
-      <c r="I12">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
-      </c>
       <c r="J12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -813,33 +862,37 @@
         <v>0.24</v>
       </c>
       <c r="C13">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>2.7599999999999971</v>
       </c>
       <c r="D13">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F13">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G13">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H13">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I13">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J13">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K13">
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -847,33 +900,37 @@
         <v>0.24</v>
       </c>
       <c r="C14">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>2.5199999999999969</v>
       </c>
       <c r="D14">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F14">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G14">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H14">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I14">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J14">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K14">
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -881,33 +938,37 @@
         <v>0.12</v>
       </c>
       <c r="C15">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>2.2799999999999967</v>
       </c>
       <c r="D15">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F15">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G15">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H15">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I15">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J15">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K15">
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -915,33 +976,37 @@
         <v>0.12</v>
       </c>
       <c r="C16">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>2.1599999999999966</v>
       </c>
       <c r="D16">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F16">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G16">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H16">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I16">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J16">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K16">
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -949,33 +1014,37 @@
         <v>0.12</v>
       </c>
       <c r="C17">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>2.0399999999999965</v>
       </c>
       <c r="D17">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F17">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G17">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H17">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I17">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J17">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K17">
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -983,33 +1052,37 @@
         <v>0.12</v>
       </c>
       <c r="C18">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>1.9199999999999964</v>
       </c>
       <c r="D18">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F18">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G18">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H18">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I18">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J18">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K18">
         <v>-1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1017,33 +1090,37 @@
         <v>0.12</v>
       </c>
       <c r="C19">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>1.7999999999999963</v>
       </c>
       <c r="D19">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F19">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G19">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H19">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I19">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J19">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K19">
         <v>-1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1051,33 +1128,37 @@
         <v>0.12</v>
       </c>
       <c r="C20">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>1.6799999999999962</v>
       </c>
       <c r="D20">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F20">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G20">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H20">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I20">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J20">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K20">
         <v>-1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1085,33 +1166,37 @@
         <v>0.12</v>
       </c>
       <c r="C21">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>1.5599999999999961</v>
       </c>
       <c r="D21">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E21">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F21">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G21">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H21">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I21">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J21">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K21">
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1119,33 +1204,37 @@
         <v>0.12</v>
       </c>
       <c r="C22">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>1.4399999999999959</v>
       </c>
       <c r="D22">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F22">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G22">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H22">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I22">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J22">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K22">
         <v>-1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1153,33 +1242,37 @@
         <v>0.12</v>
       </c>
       <c r="C23">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>1.3199999999999958</v>
       </c>
       <c r="D23">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F23">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G23">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H23">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I23">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J23">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K23">
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1187,33 +1280,37 @@
         <v>0.12</v>
       </c>
       <c r="C24">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>1.1999999999999957</v>
       </c>
       <c r="D24">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F24">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G24">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H24">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I24">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J24">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K24">
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1221,33 +1318,37 @@
         <v>0.12</v>
       </c>
       <c r="C25">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>1.0799999999999956</v>
       </c>
       <c r="D25">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E25">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F25">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G25">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H25">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I25">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K25">
         <v>-1</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1255,33 +1356,37 @@
         <v>0.12</v>
       </c>
       <c r="C26">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>0.95999999999999563</v>
       </c>
       <c r="D26">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E26">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F26">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G26">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H26">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I26">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J26">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K26">
         <v>-1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1289,33 +1394,37 @@
         <v>0.12</v>
       </c>
       <c r="C27">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>0.83999999999999564</v>
       </c>
       <c r="D27">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E27">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F27">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G27">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H27">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I27">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J27">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K27">
         <v>-1</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1323,33 +1432,37 @@
         <v>0.12</v>
       </c>
       <c r="C28">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>0.71999999999999564</v>
       </c>
       <c r="D28">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E28">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F28">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G28">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H28">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I28">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J28">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K28">
         <v>-1</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1357,33 +1470,37 @@
         <v>0.12</v>
       </c>
       <c r="C29">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>0.59999999999999565</v>
       </c>
       <c r="D29">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E29">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F29">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G29">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H29">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I29">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J29">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K29">
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1391,33 +1508,37 @@
         <v>0.12</v>
       </c>
       <c r="C30">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>0.47999999999999565</v>
       </c>
       <c r="D30">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E30">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F30">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G30">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H30">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I30">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J30">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K30">
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1425,33 +1546,37 @@
         <v>0.12</v>
       </c>
       <c r="C31">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>0.35999999999999566</v>
       </c>
       <c r="D31">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E31">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F31">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G31">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H31">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I31">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J31">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K31">
         <v>-1</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1459,33 +1584,37 @@
         <v>0.12</v>
       </c>
       <c r="C32">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>0.23999999999999566</v>
       </c>
       <c r="D32">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E32">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F32">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G32">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H32">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I32">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J32">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K32">
         <v>-1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1493,33 +1622,37 @@
         <v>0.12</v>
       </c>
       <c r="C33">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>0.11999999999999567</v>
       </c>
       <c r="D33">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E33">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F33">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G33">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H33">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I33">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J33">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K33">
         <v>-1</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1527,33 +1660,36 @@
         <v>0.12</v>
       </c>
       <c r="C34">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D34">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E34">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F34">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G34">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H34">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I34">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J34">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K34">
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1561,33 +1697,37 @@
         <v>0.12</v>
       </c>
       <c r="C35">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>-0.12</v>
       </c>
       <c r="D35">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E35">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F35">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G35">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H35">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I35">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J35">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K35">
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1595,33 +1735,37 @@
         <v>0.12</v>
       </c>
       <c r="C36">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>-0.24</v>
       </c>
       <c r="D36">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E36">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F36">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G36">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H36">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I36">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1629,33 +1773,37 @@
         <v>0.12</v>
       </c>
       <c r="C37">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>-0.36</v>
       </c>
       <c r="D37">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E37">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F37">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G37">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H37">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I37">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1663,33 +1811,37 @@
         <v>0.12</v>
       </c>
       <c r="C38">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>-0.48</v>
       </c>
       <c r="D38">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E38">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F38">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G38">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H38">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I38">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1697,33 +1849,37 @@
         <v>0.12</v>
       </c>
       <c r="C39">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>-0.6</v>
       </c>
       <c r="D39">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E39">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F39">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G39">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H39">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I39">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1731,33 +1887,37 @@
         <v>0.12</v>
       </c>
       <c r="C40">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>-0.72</v>
       </c>
       <c r="D40">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E40">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F40">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G40">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H40">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I40">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1765,33 +1925,37 @@
         <v>0.12</v>
       </c>
       <c r="C41">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>-0.84</v>
       </c>
       <c r="D41">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E41">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F41">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G41">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H41">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I41">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1799,33 +1963,37 @@
         <v>0.12</v>
       </c>
       <c r="C42">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>-0.96</v>
       </c>
       <c r="D42">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E42">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F42">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G42">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H42">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I42">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1833,33 +2001,37 @@
         <v>0.12</v>
       </c>
       <c r="C43">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>-1.08</v>
       </c>
       <c r="D43">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E43">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F43">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G43">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H43">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I43">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1867,33 +2039,37 @@
         <v>0.12</v>
       </c>
       <c r="C44">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>-1.2000000000000002</v>
       </c>
       <c r="D44">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E44">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F44">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G44">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H44">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I44">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1901,33 +2077,37 @@
         <v>0.12</v>
       </c>
       <c r="C45">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>-1.3200000000000003</v>
       </c>
       <c r="D45">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E45">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F45">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G45">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H45">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I45">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1935,33 +2115,37 @@
         <v>0.12</v>
       </c>
       <c r="C46">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>-1.4400000000000004</v>
       </c>
       <c r="D46">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E46">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F46">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G46">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H46">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I46">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1969,33 +2153,37 @@
         <v>0.16</v>
       </c>
       <c r="C47">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>-1.5600000000000005</v>
       </c>
       <c r="D47">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E47">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F47">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G47">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H47">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I47">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2003,33 +2191,37 @@
         <v>0.08</v>
       </c>
       <c r="C48">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>-1.7200000000000004</v>
       </c>
       <c r="D48">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E48">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F48">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G48">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H48">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I48">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2037,33 +2229,37 @@
         <v>0.12</v>
       </c>
       <c r="C49">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>-1.8000000000000005</v>
       </c>
       <c r="D49">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E49">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F49">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G49">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H49">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I49">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2071,33 +2267,37 @@
         <v>0.12</v>
       </c>
       <c r="C50">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>-1.9200000000000004</v>
       </c>
       <c r="D50">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E50">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F50">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G50">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H50">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I50">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2105,33 +2305,37 @@
         <v>0.12</v>
       </c>
       <c r="C51">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>-2.0400000000000005</v>
       </c>
       <c r="D51">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E51">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F51">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G51">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H51">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I51">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2139,33 +2343,37 @@
         <v>0.12</v>
       </c>
       <c r="C52">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>-2.1600000000000006</v>
       </c>
       <c r="D52">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E52">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F52">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G52">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H52">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I52">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2173,33 +2381,37 @@
         <v>0.12</v>
       </c>
       <c r="C53">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>-2.2800000000000007</v>
       </c>
       <c r="D53">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E53">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F53">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G53">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H53">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I53">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2207,33 +2419,37 @@
         <v>0.12</v>
       </c>
       <c r="C54">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>-2.4000000000000008</v>
       </c>
       <c r="D54">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E54">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F54">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G54">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H54">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I54">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2241,33 +2457,37 @@
         <v>0.12</v>
       </c>
       <c r="C55">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>-2.5200000000000009</v>
       </c>
       <c r="D55">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E55">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F55">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G55">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H55">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I55">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2275,33 +2495,37 @@
         <v>0.12</v>
       </c>
       <c r="C56">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>-2.640000000000001</v>
       </c>
       <c r="D56">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E56">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F56">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G56">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H56">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I56">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2309,33 +2533,37 @@
         <v>0.16</v>
       </c>
       <c r="C57">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>-2.7600000000000011</v>
       </c>
       <c r="D57">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E57">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F57">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G57">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H57">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I57">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2343,33 +2571,37 @@
         <v>0.08</v>
       </c>
       <c r="C58">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>-2.9200000000000013</v>
       </c>
       <c r="D58">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E58">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F58">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G58">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H58">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I58">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2377,33 +2609,37 @@
         <v>0.12</v>
       </c>
       <c r="C59">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>-3.0000000000000013</v>
       </c>
       <c r="D59">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E59">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F59">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G59">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H59">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I59">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2411,33 +2647,37 @@
         <v>0.12</v>
       </c>
       <c r="C60">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>-3.1200000000000014</v>
       </c>
       <c r="D60">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E60">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F60">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G60">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H60">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I60">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2445,29 +2685,33 @@
         <v>0.12</v>
       </c>
       <c r="C61">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>-3.2400000000000015</v>
       </c>
       <c r="D61">
-        <v>0.875</v>
+        <v>16</v>
       </c>
       <c r="E61">
-        <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>0.875</v>
       </c>
       <c r="F61">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17.75</v>
       </c>
       <c r="G61">
-        <v>0.875</v>
+        <v>11</v>
       </c>
       <c r="H61">
-        <v>4.625</v>
+        <v>0.875</v>
       </c>
       <c r="I61">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.625</v>
       </c>
       <c r="J61">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="K61">
         <v>0</v>
       </c>
     </row>

</xml_diff>